<commit_message>
Load Excel Data done
</commit_message>
<xml_diff>
--- a/offset.xlsx
+++ b/offset.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sungjinkim\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_26_python\1_repo\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6418390B-F156-4858-8762-D46BB38A6382}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D712C88D-152D-4E24-86E7-E924BAE04BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="-108" windowWidth="21864" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-49740" yWindow="5745" windowWidth="17070" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -381,8 +381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -426,10 +426,10 @@
         <v>6000000000</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>-0.1</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>-50</v>
       </c>
       <c r="D3">
         <v>28</v>
@@ -440,10 +440,10 @@
         <v>7000000000</v>
       </c>
       <c r="B4">
-        <v>0.2</v>
+        <v>-0.2</v>
       </c>
       <c r="C4">
-        <v>50.1</v>
+        <v>-50.1</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -451,10 +451,10 @@
         <v>8000000000</v>
       </c>
       <c r="B5">
-        <v>0.3</v>
+        <v>-0.3</v>
       </c>
       <c r="C5">
-        <v>50.2</v>
+        <v>-50.2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -462,10 +462,10 @@
         <v>9000000000</v>
       </c>
       <c r="B6">
-        <v>0.4</v>
+        <v>-0.4</v>
       </c>
       <c r="C6">
-        <v>50.3</v>
+        <v>-50.3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -473,10 +473,10 @@
         <v>10000000000</v>
       </c>
       <c r="B7">
-        <v>0.5</v>
+        <v>-0.5</v>
       </c>
       <c r="C7">
-        <v>50.4</v>
+        <v>-50.4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -484,10 +484,10 @@
         <v>11000000000</v>
       </c>
       <c r="B8">
-        <v>0.6</v>
+        <v>-0.6</v>
       </c>
       <c r="C8">
-        <v>50.5</v>
+        <v>-50.5</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -495,10 +495,10 @@
         <v>12000000000</v>
       </c>
       <c r="B9">
-        <v>0.7</v>
+        <v>-0.7</v>
       </c>
       <c r="C9">
-        <v>50.6</v>
+        <v>-50.6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -506,10 +506,10 @@
         <v>13000000000</v>
       </c>
       <c r="B10">
-        <v>0.8</v>
+        <v>-0.8</v>
       </c>
       <c r="C10">
-        <v>50.7</v>
+        <v>-50.7</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -517,10 +517,10 @@
         <v>14000000000</v>
       </c>
       <c r="B11">
-        <v>0.9</v>
+        <v>-0.9</v>
       </c>
       <c r="C11">
-        <v>50.8</v>
+        <v>-50.8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -528,10 +528,10 @@
         <v>15000000000</v>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="C12">
-        <v>50.9</v>
+        <v>-50.9</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
@@ -539,10 +539,10 @@
         <v>16000000000</v>
       </c>
       <c r="B13">
-        <v>1.1000000000000001</v>
+        <v>-1.1000000000000001</v>
       </c>
       <c r="C13">
-        <v>51</v>
+        <v>-51</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.4">
@@ -550,10 +550,10 @@
         <v>17000000000</v>
       </c>
       <c r="B14">
-        <v>1.2</v>
+        <v>-1.2</v>
       </c>
       <c r="C14">
-        <v>51.1</v>
+        <v>-51.1</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.4">
@@ -561,10 +561,10 @@
         <v>18000000000</v>
       </c>
       <c r="B15">
-        <v>1.3</v>
+        <v>-1.3</v>
       </c>
       <c r="C15">
-        <v>51.2</v>
+        <v>-51.2</v>
       </c>
     </row>
   </sheetData>
@@ -591,7 +591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F59CA7F-3583-4794-9779-641ADAE5C924}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add name, aging time, power atr dialog register
</commit_message>
<xml_diff>
--- a/offset.xlsx
+++ b/offset.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_26_python\1_repo\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D712C88D-152D-4E24-86E7-E924BAE04BF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C564D59F-EB89-4DB9-B85E-CB2AF181C2AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-49740" yWindow="5745" windowWidth="17070" windowHeight="6000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1284" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>frequency</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -54,6 +54,14 @@
   </si>
   <si>
     <t>Power Voltage</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sec</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Start aging</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -379,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -391,9 +399,10 @@
     <col min="2" max="2" width="11.19921875" customWidth="1"/>
     <col min="3" max="3" width="12.69921875" customWidth="1"/>
     <col min="4" max="4" width="14.59765625" customWidth="1"/>
+    <col min="5" max="5" width="10.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -406,8 +415,11 @@
       <c r="D1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -420,8 +432,11 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>6000000000</v>
       </c>
@@ -434,8 +449,11 @@
       <c r="D3">
         <v>28</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>7000000000</v>
       </c>
@@ -446,7 +464,7 @@
         <v>-50.1</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>8000000000</v>
       </c>
@@ -457,7 +475,7 @@
         <v>-50.2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>9000000000</v>
       </c>
@@ -468,7 +486,7 @@
         <v>-50.3</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>10000000000</v>
       </c>
@@ -479,7 +497,7 @@
         <v>-50.4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>11000000000</v>
       </c>
@@ -490,7 +508,7 @@
         <v>-50.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>12000000000</v>
       </c>
@@ -501,7 +519,7 @@
         <v>-50.6</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>13000000000</v>
       </c>
@@ -512,7 +530,7 @@
         <v>-50.7</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>14000000000</v>
       </c>
@@ -523,7 +541,7 @@
         <v>-50.8</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>15000000000</v>
       </c>
@@ -534,7 +552,7 @@
         <v>-50.9</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>16000000000</v>
       </c>
@@ -545,7 +563,7 @@
         <v>-51</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>17000000000</v>
       </c>
@@ -556,7 +574,7 @@
         <v>-51.1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>18000000000</v>
       </c>

</xml_diff>

<commit_message>
input output offset search depend user frequency complished
</commit_message>
<xml_diff>
--- a/offset.xlsx
+++ b/offset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_26_python\1_repo\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{393598E3-3268-4649-9C34-A1E8F46B8C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA586D5-9999-41E2-BAC1-88AF589FBA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1284" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
   <si>
     <t>frequency</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -80,14 +80,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>unit ex</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -104,10 +96,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>power source voltage data</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>source generate communication data</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -153,6 +141,94 @@
   </si>
   <si>
     <t>Output offset</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Select Freq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GHz</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Current Limit</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power meter probe Channel</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power supply current limit data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>power supply voltage data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">power meter probe number </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fixed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>B</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>D</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>E</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>F</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>G</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>I</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>J</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unit(row = 2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name(row = 1)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -485,50 +561,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="13.09765625" customWidth="1"/>
-    <col min="2" max="2" width="11.19921875" customWidth="1"/>
-    <col min="3" max="3" width="12.69921875" customWidth="1"/>
-    <col min="4" max="4" width="14.59765625" customWidth="1"/>
-    <col min="5" max="5" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.69921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.59765625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -542,19 +631,28 @@
         <v>4</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>6000000000</v>
       </c>
@@ -568,19 +666,28 @@
         <v>28</v>
       </c>
       <c r="E3">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="F3">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>13</v>
+      </c>
+      <c r="K3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>7000000000</v>
       </c>
@@ -590,8 +697,11 @@
       <c r="C4">
         <v>50.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K4">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>8000000000</v>
       </c>
@@ -601,8 +711,11 @@
       <c r="C5">
         <v>50.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>9000000000</v>
       </c>
@@ -612,8 +725,11 @@
       <c r="C6">
         <v>50.3</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K6">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>10000000000</v>
       </c>
@@ -623,8 +739,11 @@
       <c r="C7">
         <v>50.4</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>11000000000</v>
       </c>
@@ -634,8 +753,11 @@
       <c r="C8">
         <v>50.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K8">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>12000000000</v>
       </c>
@@ -645,8 +767,11 @@
       <c r="C9">
         <v>50.6</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>13000000000</v>
       </c>
@@ -656,8 +781,11 @@
       <c r="C10">
         <v>50.7</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K10">
+        <v>9.5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>14000000000</v>
       </c>
@@ -667,8 +795,11 @@
       <c r="C11">
         <v>50.8</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>15000000000</v>
       </c>
@@ -678,8 +809,11 @@
       <c r="C12">
         <v>50.9</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K12">
+        <v>10.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>16000000000</v>
       </c>
@@ -689,8 +823,11 @@
       <c r="C13">
         <v>51</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
+      <c r="K13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>17000000000</v>
       </c>
@@ -701,7 +838,7 @@
         <v>51.1</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>18000000000</v>
       </c>
@@ -721,136 +858,207 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200DA2CE-D9F0-4A24-84A6-96B5876B084D}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="34.69921875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.69921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.3984375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.3984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="32.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="E1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="E11" t="s">
         <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
p1 prototype done but it needs limit.
</commit_message>
<xml_diff>
--- a/offset.xlsx
+++ b/offset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_26_python\1_repo\pythonProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CA586D5-9999-41E2-BAC1-88AF589FBA8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4831CBF2-55C4-42AB-8086-FB871C66B52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1284" yWindow="-108" windowWidth="21864" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1392" yWindow="1188" windowWidth="20292" windowHeight="11772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="56">
   <si>
     <t>frequency</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -229,6 +229,26 @@
   </si>
   <si>
     <t>name(row = 1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>dBm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Psat input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Overdrive input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ATR start input dBm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -561,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -580,9 +600,12 @@
     <col min="9" max="9" width="12.59765625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -616,8 +639,20 @@
       <c r="K1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -651,8 +686,20 @@
       <c r="K2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L2" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>6000000000</v>
       </c>
@@ -675,19 +722,31 @@
         <v>1</v>
       </c>
       <c r="H3">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J3">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="K3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.4">
+      <c r="L3">
+        <v>-20</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>8</v>
+      </c>
+      <c r="O3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>7000000000</v>
       </c>
@@ -701,7 +760,7 @@
         <v>6.5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>8000000000</v>
       </c>
@@ -715,7 +774,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>9000000000</v>
       </c>
@@ -729,7 +788,7 @@
         <v>7.5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>10000000000</v>
       </c>
@@ -743,7 +802,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>11000000000</v>
       </c>
@@ -757,7 +816,7 @@
         <v>8.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>12000000000</v>
       </c>
@@ -771,7 +830,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>13000000000</v>
       </c>
@@ -785,7 +844,7 @@
         <v>9.5</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>14000000000</v>
       </c>
@@ -799,7 +858,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>15000000000</v>
       </c>
@@ -813,7 +872,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>16000000000</v>
       </c>
@@ -827,7 +886,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>17000000000</v>
       </c>
@@ -838,7 +897,7 @@
         <v>51.1</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>18000000000</v>
       </c>

</xml_diff>